<commit_message>
Programa envia mensajes con formato que definio Jorge, se espera el inicio del desarrollo de la interfaz grafica
</commit_message>
<xml_diff>
--- a/Contactos.xlsx
+++ b/Contactos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -31,19 +31,13 @@
     <t xml:space="preserve">Genero</t>
   </si>
   <si>
-    <t xml:space="preserve">Gloria Velez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hna</t>
+    <t xml:space="preserve">Sebastian Romero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hno</t>
   </si>
   <si>
     <t xml:space="preserve">Pablo Romero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sebastian Romero</t>
   </si>
 </sst>
 </file>
@@ -133,16 +127,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -219,69 +217,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.43359375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="15.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>573222006394</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="1" t="n">
+        <v>573138793438</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>573114524438</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>573138793438</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="2"/>
+      <c r="D8" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Interfaz funcionando correctamente, solo nos falta configurar el tema del mensaje
</commit_message>
<xml_diff>
--- a/Contactos.xlsx
+++ b/Contactos.xlsx
@@ -224,7 +224,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.43359375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -266,7 +266,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0"/>
+      <c r="B4" s="0"/>
+      <c r="C4" s="0"/>
+    </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="3"/>

</xml_diff>

<commit_message>
Interfaz funcionando, ahora iniciamos pruebas con caracteres especiales
</commit_message>
<xml_diff>
--- a/Contactos.xlsx
+++ b/Contactos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -34,10 +34,7 @@
     <t xml:space="preserve">Sebastian Romero</t>
   </si>
   <si>
-    <t xml:space="preserve">Hno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pablo Romero</t>
+    <t xml:space="preserve">Sr</t>
   </si>
 </sst>
 </file>
@@ -224,7 +221,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.43359375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -255,22 +252,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>573114524438</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0"/>
-      <c r="B4" s="0"/>
-      <c r="C4" s="0"/>
-    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="3"/>

</xml_diff>

<commit_message>
version 2.0, funciona todo perfecto, se va a intentar automatizar la instalacion, junto con mejorar la interfaz grafica para envio de imagenes y videos
</commit_message>
<xml_diff>
--- a/Contactos.xlsx
+++ b/Contactos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">Sr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pablo Romero</t>
   </si>
 </sst>
 </file>
@@ -124,7 +127,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -134,6 +137,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -221,7 +228,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.43359375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -252,11 +259,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>573114524438</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D7" s="3"/>
+    </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="3"/>
+      <c r="D8" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Se envia correctamente mensaje con formulario, ahora solo falta pulir el tema de los envios con imagenes o videos
</commit_message>
<xml_diff>
--- a/Contactos.xlsx
+++ b/Contactos.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Sebastian Romero</t>
   </si>
   <si>
-    <t xml:space="preserve">Sr</t>
+    <t xml:space="preserve">Hno</t>
   </si>
   <si>
     <t xml:space="preserve">Pablo Romero</t>
@@ -127,7 +127,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -137,10 +137,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -225,10 +221,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.43359375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -272,12 +268,16 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="4"/>
-    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Programa funcionando para enviar fotos y videos
</commit_message>
<xml_diff>
--- a/Contactos.xlsx
+++ b/Contactos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -31,13 +31,10 @@
     <t xml:space="preserve">Genero</t>
   </si>
   <si>
-    <t xml:space="preserve">Sebastian Romero</t>
+    <t xml:space="preserve">Juan Sebastian Romero Velez</t>
   </si>
   <si>
     <t xml:space="preserve">Hno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pablo Romero</t>
   </si>
 </sst>
 </file>
@@ -47,7 +44,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -71,11 +68,25 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <u val="single"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -93,7 +104,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -101,6 +112,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -127,7 +145,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -136,11 +154,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -221,15 +255,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.43359375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.43359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="15.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12"/>
   </cols>
   <sheetData>
@@ -245,39 +280,165 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="3" t="n">
         <v>573138793438</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>573114524438</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+    </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="3"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Se hizo una actualizacion, pues la interfaz de WhatsApp Web cambio, el cambio estuvo a la hora de adjuntar un video o imagen
</commit_message>
<xml_diff>
--- a/Contactos.xlsx
+++ b/Contactos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t xml:space="preserve">Hno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pablo Romero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caballero</t>
   </si>
 </sst>
 </file>
@@ -258,7 +264,7 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.43359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -291,9 +297,15 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>573114524438</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="D3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Nueva actualización lista, se trato que ahora las imagenes y videos sean enviado de la mejor manera
</commit_message>
<xml_diff>
--- a/Contactos.xlsx
+++ b/Contactos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t xml:space="preserve">Caballero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sebastian Romero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joven</t>
   </si>
 </sst>
 </file>
@@ -264,7 +270,7 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.43359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -309,9 +315,15 @@
       <c r="D3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4"/>
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>573138793438</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>

</xml_diff>

<commit_message>
Actualización de los archivos setup con la intencion que el desarrollador pueda instalar todas las dependencias de manera mas facil y comoda sin importar si programa desde Windows o Linux
</commit_message>
<xml_diff>
--- a/Contactos.xlsx
+++ b/Contactos.xlsx
@@ -31,19 +31,19 @@
     <t xml:space="preserve">Genero</t>
   </si>
   <si>
-    <t xml:space="preserve">Juan Sebastian Romero Velez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pablo Romero</t>
+    <t xml:space="preserve">Yeison Farfan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Johan Fonsecha</t>
   </si>
   <si>
     <t xml:space="preserve">Caballero</t>
   </si>
   <si>
-    <t xml:space="preserve">Sebastian Romero</t>
+    <t xml:space="preserve">Sebastian Martinez</t>
   </si>
   <si>
     <t xml:space="preserve">Joven</t>
@@ -263,17 +263,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.43359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.22"/>
@@ -296,7 +296,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="n">
-        <v>573138793438</v>
+        <v>573208539538</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -307,7 +307,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>573114524438</v>
+        <v>573208113787</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>6</v>
@@ -319,7 +319,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>573138793438</v>
+        <v>573138600528</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>8</v>

</xml_diff>